<commit_message>
fix for in line alarm comments
</commit_message>
<xml_diff>
--- a/lighterFluid/heavierFluidOutputs/lnlBackConvert.xlsx
+++ b/lighterFluid/heavierFluidOutputs/lnlBackConvert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoghanoc\source\repos\lighterFluid\lighterFluid\heavierFluidOutputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBC2073-1F90-44D9-A898-3F2FF112953E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D602775E-1B24-45FB-8DB1-2608831FA1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1965" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fun_core" sheetId="1" r:id="rId1"/>

</xml_diff>